<commit_message>
update the GPP evaluation for sites
</commit_message>
<xml_diff>
--- a/data-raw/site_info_more_details.xlsx
+++ b/data-raw/site_info_more_details.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20390"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48CE218A-9D44-4840-911E-9BB71CD2BAD3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCFA59FC-A13D-4D2A-AFD7-A0C589B3879F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -459,7 +459,7 @@
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
update the gpp overestimation
</commit_message>
<xml_diff>
--- a/data-raw/site_info_more_details.xlsx
+++ b/data-raw/site_info_more_details.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20390"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20391"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCFA59FC-A13D-4D2A-AFD7-A0C589B3879F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A78603-0531-422B-9D0E-200E6122A8B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="site_info" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
   <si>
     <t>Sitename</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Physio. &amp; Hydro. measure.</t>
   </si>
   <si>
-    <t>Other avai. measurements</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
@@ -112,9 +109,6 @@
     <t>thomas.gruenwald@tu-dresden.de</t>
   </si>
   <si>
-    <t>Timo Vesala, Juan Porcar-Castell</t>
-  </si>
-  <si>
     <t>Michiel van der Molen</t>
   </si>
   <si>
@@ -128,6 +122,27 @@
   </si>
   <si>
     <t>MAP</t>
+  </si>
+  <si>
+    <t>Avai. C fluxes from</t>
+  </si>
+  <si>
+    <t>1996-</t>
+  </si>
+  <si>
+    <t>1997-</t>
+  </si>
+  <si>
+    <t>Other avai. Measure.</t>
+  </si>
+  <si>
+    <t>PhenoCam. measure.</t>
+  </si>
+  <si>
+    <t>Timo Vesala, Albert Porcar-Castell, Anna Lintunen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sapflow, dendrometer </t>
   </si>
 </sst>
 </file>
@@ -456,29 +471,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="4.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="4.77734375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="31.26953125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="52.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="44.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -495,39 +512,45 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" t="s">
         <v>33</v>
-      </c>
-      <c r="G1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H1" t="s">
-        <v>35</v>
       </c>
       <c r="I1" t="s">
         <v>5</v>
       </c>
       <c r="J1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N1" t="s">
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2">
         <v>24.3</v>
@@ -536,10 +559,10 @@
         <v>61.85</v>
       </c>
       <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
         <v>18</v>
-      </c>
-      <c r="F2" t="s">
-        <v>19</v>
       </c>
       <c r="G2">
         <v>3.8</v>
@@ -548,30 +571,36 @@
         <v>709</v>
       </c>
       <c r="I2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J2" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="K2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="M2" t="s">
-        <v>30</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
+      </c>
+      <c r="N2" t="s">
+        <v>40</v>
+      </c>
+      <c r="O2" t="s">
+        <v>39</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3">
         <v>5.74</v>
@@ -580,10 +609,10 @@
         <v>52.17</v>
       </c>
       <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
         <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
       </c>
       <c r="G3">
         <v>9.8000000000000007</v>
@@ -592,24 +621,27 @@
         <v>786</v>
       </c>
       <c r="I3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" t="s">
-        <v>24</v>
-      </c>
-      <c r="M3" t="s">
-        <v>31</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
+      </c>
+      <c r="J3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4">
         <v>13.57</v>
@@ -618,10 +650,10 @@
         <v>50.96</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G4">
         <v>8.1999999999999993</v>
@@ -630,21 +662,30 @@
         <v>843</v>
       </c>
       <c r="I4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4" t="s">
         <v>22</v>
       </c>
-      <c r="M4" t="s">
-        <v>32</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>29</v>
+      <c r="N4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O4" t="s">
+        <v>30</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5">
         <v>9.85</v>
@@ -653,10 +694,10 @@
         <v>46.82</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G5">
         <v>2.8</v>
@@ -665,14 +706,20 @@
         <v>1062</v>
       </c>
       <c r="I5" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="J5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K5" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N2" r:id="rId1" display="joan.porcar@helsinki.fi;timo.vesala@helsinki.fi     " xr:uid="{C07FFC51-6677-48FB-8E53-9B6469100213}"/>
-    <hyperlink ref="N3" r:id="rId2" xr:uid="{23E81624-560E-4ED6-8EAD-56C4D9109C80}"/>
-    <hyperlink ref="N4" r:id="rId3" xr:uid="{226806B0-2419-4462-876C-4741C79C3C16}"/>
+    <hyperlink ref="P2" r:id="rId1" display="joan.porcar@helsinki.fi;timo.vesala@helsinki.fi     " xr:uid="{C07FFC51-6677-48FB-8E53-9B6469100213}"/>
+    <hyperlink ref="P3" r:id="rId2" xr:uid="{23E81624-560E-4ED6-8EAD-56C4D9109C80}"/>
+    <hyperlink ref="P4" r:id="rId3" xr:uid="{226806B0-2419-4462-876C-4741C79C3C16}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>